<commit_message>
SIFT detector with ORB descriptor
</commit_message>
<xml_diff>
--- a/camera/less5_2d_tracking/2d_feat_tracking/results/features_comparison.xlsx
+++ b/camera/less5_2d_tracking/2d_feat_tracking/results/features_comparison.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="79">
   <si>
     <t>SL.No</t>
   </si>
@@ -19,7 +19,7 @@
     <t>Keypoints Method</t>
   </si>
   <si>
-    <t>Counts (for front vehicle)</t>
+    <t>Counts (for front vehicle on each image)</t>
   </si>
   <si>
     <t>Timing (ms)</t>
@@ -142,7 +142,7 @@
     <t>70 - 90</t>
   </si>
   <si>
-    <t>Memory Error</t>
+    <t>80 - 100</t>
   </si>
   <si>
     <t>60 - 80</t>
@@ -179,9 +179,6 @@
   </si>
   <si>
     <t>30 - 60</t>
-  </si>
-  <si>
-    <t>80 - 100</t>
   </si>
   <si>
     <t>130 - 150</t>
@@ -414,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -428,6 +425,9 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -486,6 +486,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="13" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="14" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -719,6 +722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -764,10 +768,10 @@
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="2"/>
@@ -778,16 +782,16 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4">
-      <c r="A4" s="6">
+      <c r="A4" s="7">
         <v>1.0</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="2"/>
@@ -798,16 +802,16 @@
       <c r="J4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="6">
+      <c r="A5" s="7">
         <v>2.0</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="2"/>
@@ -818,16 +822,16 @@
       <c r="J5" s="1"/>
     </row>
     <row r="6">
-      <c r="A6" s="6">
+      <c r="A6" s="7">
         <v>3.0</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="2"/>
@@ -838,16 +842,16 @@
       <c r="J6" s="1"/>
     </row>
     <row r="7">
-      <c r="A7" s="6">
+      <c r="A7" s="7">
         <v>4.0</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="2"/>
@@ -858,16 +862,16 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8">
-      <c r="A8" s="6">
+      <c r="A8" s="7">
         <v>5.0</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="2"/>
@@ -878,16 +882,16 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9">
-      <c r="A9" s="6">
+      <c r="A9" s="7">
         <v>6.0</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="9" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="2"/>
@@ -898,16 +902,16 @@
       <c r="J9" s="1"/>
     </row>
     <row r="10">
-      <c r="A10" s="9">
+      <c r="A10" s="10">
         <v>7.0</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="12" t="s">
         <v>24</v>
       </c>
       <c r="E10" s="2"/>
@@ -922,7 +926,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="13" t="s">
         <v>25</v>
       </c>
       <c r="I11" s="1"/>
@@ -932,57 +936,57 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14" t="s">
+      <c r="D12" s="14"/>
+      <c r="E12" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="14" t="s">
+      <c r="I12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="15" t="s">
+      <c r="J12" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="K12" s="16" t="s">
+      <c r="K12" s="17" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="20" t="s">
+      <c r="B13" s="19"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="G13" s="21" t="s">
+      <c r="G13" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="H13" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="I13" s="21" t="s">
+      <c r="I13" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="J13" s="21" t="s">
+      <c r="J13" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="K13" s="22"/>
+      <c r="K13" s="23"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -1001,30 +1005,30 @@
       <c r="AA13" s="1"/>
     </row>
     <row r="14">
-      <c r="A14" s="23"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="20" t="s">
+      <c r="A14" s="24"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="21" t="s">
+      <c r="G14" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="21" t="s">
+      <c r="H14" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="21" t="s">
+      <c r="I14" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J14" s="21" t="s">
+      <c r="J14" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="K14" s="22"/>
+      <c r="K14" s="23"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -1043,30 +1047,30 @@
       <c r="AA14" s="1"/>
     </row>
     <row r="15">
-      <c r="A15" s="23"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="20" t="s">
+      <c r="A15" s="24"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="E15" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="21" t="s">
+      <c r="G15" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="H15" s="21" t="s">
+      <c r="H15" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="I15" s="21" t="s">
+      <c r="I15" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="J15" s="21" t="s">
+      <c r="J15" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="K15" s="22"/>
+      <c r="K15" s="23"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -1085,30 +1089,30 @@
       <c r="AA15" s="1"/>
     </row>
     <row r="16">
-      <c r="A16" s="23"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="20" t="s">
+      <c r="A16" s="24"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="G16" s="21" t="s">
+      <c r="G16" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="H16" s="21" t="s">
+      <c r="H16" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="I16" s="21" t="s">
+      <c r="I16" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="J16" s="21" t="s">
+      <c r="J16" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="K16" s="22"/>
+      <c r="K16" s="23"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -1127,30 +1131,30 @@
       <c r="AA16" s="1"/>
     </row>
     <row r="17">
-      <c r="A17" s="23"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="20" t="s">
+      <c r="A17" s="24"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E17" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="F17" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="G17" s="21" t="s">
+      <c r="G17" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="H17" s="21" t="s">
+      <c r="H17" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="21" t="s">
+      <c r="I17" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="J17" s="21" t="s">
+      <c r="J17" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="K17" s="22"/>
+      <c r="K17" s="23"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
@@ -1169,30 +1173,30 @@
       <c r="AA17" s="1"/>
     </row>
     <row r="18">
-      <c r="A18" s="23"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="20" t="s">
+      <c r="A18" s="24"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="E18" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="F18" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="G18" s="21" t="s">
+      <c r="G18" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H18" s="21" t="s">
+      <c r="H18" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="I18" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="J18" s="21" t="s">
+      <c r="I18" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="J18" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="K18" s="22"/>
+      <c r="K18" s="23"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
@@ -1211,30 +1215,30 @@
       <c r="AA18" s="1"/>
     </row>
     <row r="19">
-      <c r="A19" s="23"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="20" t="s">
+      <c r="A19" s="24"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="E19" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="F19" s="21" t="s">
+      <c r="G19" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G19" s="21" t="s">
+      <c r="H19" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="H19" s="21" t="s">
+      <c r="I19" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="I19" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="J19" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="K19" s="22"/>
+      <c r="J19" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="K19" s="23"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
@@ -1253,19 +1257,19 @@
       <c r="AA19" s="1"/>
     </row>
     <row r="20">
-      <c r="A20" s="23"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="1"/>
+      <c r="A20" s="24"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="28"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
@@ -1283,18 +1287,18 @@
       <c r="AA20" s="1"/>
     </row>
     <row r="21">
-      <c r="A21" s="23"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="30"/>
+      <c r="A21" s="24"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="32"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -1313,28 +1317,28 @@
       <c r="AA21" s="1"/>
     </row>
     <row r="22">
-      <c r="A22" s="23"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="21" t="s">
+      <c r="A22" s="24"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="21" t="s">
+      <c r="F22" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="21" t="s">
+      <c r="G22" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="H22" s="21" t="s">
+      <c r="H22" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="I22" s="21" t="s">
+      <c r="I22" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="J22" s="21" t="s">
+      <c r="J22" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="K22" s="32" t="s">
+      <c r="K22" s="34" t="s">
         <v>28</v>
       </c>
       <c r="L22" s="1"/>
@@ -1355,30 +1359,30 @@
       <c r="AA22" s="1"/>
     </row>
     <row r="23">
-      <c r="A23" s="23"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="20" t="s">
+      <c r="A23" s="24"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="21" t="s">
+      <c r="E23" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="21" t="s">
+      <c r="F23" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G23" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="G23" s="21" t="s">
+      <c r="H23" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="I23" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="H23" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="I23" s="21" t="s">
+      <c r="J23" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="J23" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="K23" s="22"/>
+      <c r="K23" s="23"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -1397,30 +1401,30 @@
       <c r="AA23" s="1"/>
     </row>
     <row r="24">
-      <c r="A24" s="23"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="20" t="s">
+      <c r="A24" s="24"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F24" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="G24" s="21" t="s">
+      <c r="E24" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="G24" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="H24" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="I24" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="H24" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="I24" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="J24" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="K24" s="22"/>
+      <c r="J24" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="K24" s="23"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
@@ -1439,30 +1443,30 @@
       <c r="AA24" s="1"/>
     </row>
     <row r="25">
-      <c r="A25" s="23"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="20" t="s">
+      <c r="A25" s="24"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="21" t="s">
+      <c r="E25" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="G25" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="F25" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="G25" s="21" t="s">
+      <c r="H25" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="I25" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="H25" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="I25" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="J25" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="K25" s="22"/>
+      <c r="J25" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="K25" s="23"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
@@ -1481,30 +1485,30 @@
       <c r="AA25" s="1"/>
     </row>
     <row r="26">
-      <c r="A26" s="23"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="20" t="s">
+      <c r="A26" s="24"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="21" t="s">
+      <c r="E26" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="F26" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="F26" s="21" t="s">
+      <c r="G26" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="G26" s="21" t="s">
+      <c r="H26" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="I26" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="H26" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="I26" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="J26" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="K26" s="22"/>
+      <c r="J26" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="K26" s="23"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
@@ -1523,30 +1527,30 @@
       <c r="AA26" s="1"/>
     </row>
     <row r="27">
-      <c r="A27" s="23"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="20" t="s">
+      <c r="A27" s="24"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="F27" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="G27" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="H27" s="21" t="s">
+      <c r="E27" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="F27" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="G27" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="I27" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="J27" s="21" t="s">
+      <c r="I27" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="J27" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="K27" s="22"/>
+      <c r="K27" s="23"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
@@ -1565,31 +1569,31 @@
       <c r="AA27" s="1"/>
     </row>
     <row r="28">
-      <c r="A28" s="33"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="20" t="s">
+      <c r="A28" s="35"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="E28" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="F28" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="H28" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="I28" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="F28" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="G28" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="H28" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="I28" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="J28" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="K28" s="22"/>
+      <c r="J28" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="K28" s="23"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
@@ -1611,28 +1615,28 @@
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="36" t="s">
+      <c r="D29" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="21" t="s">
+      <c r="E29" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F29" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="G29" s="21" t="s">
+      <c r="F29" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="H29" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="H29" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="I29" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="J29" s="21" t="s">
+      <c r="I29" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="J29" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="K29" s="37"/>
+      <c r="K29" s="39"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
@@ -1654,8 +1658,8 @@
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="12" t="s">
-        <v>61</v>
+      <c r="D30" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="1"/>
@@ -13310,6 +13314,9 @@
     <mergeCell ref="E21:H21"/>
     <mergeCell ref="A13:C28"/>
   </mergeCells>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>